<commit_message>
Se cambiaron los metodos de programacion dinamica, y mejorada y se agrego de pow.
</commit_message>
<xml_diff>
--- a/TP2/GráficosPolinomios.xlsx
+++ b/TP2/GráficosPolinomios.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\flopez\PrograAvanzadaClaseTp\TP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaqu\Desktop\ProgramacionAvanzada\PrograAvanzadaClaseTp\TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="80" windowWidth="14120" windowHeight="5190"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14115" windowHeight="5190"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -562,7 +562,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>70746</c:v>
+                  <c:v>63293</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>68923</c:v>
@@ -726,7 +726,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -752,7 +751,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -790,7 +789,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="845111136"/>
@@ -852,7 +851,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -878,7 +876,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -910,7 +908,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="845125696"/>
@@ -951,7 +949,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1535,7 +1533,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Gráfico 8"/>
+        <xdr:cNvPr id="9" name="Gráfico 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1554,7 +1558,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1629,6 +1633,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1664,6 +1685,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1842,13 +1880,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1870,7 +1908,7 @@
       </c>
       <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -1902,7 +1940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1925,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="2">
-        <v>70746</v>
+        <v>63293</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -1934,7 +1972,7 @@
         <v>25527</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>10</v>
       </c>
@@ -1966,7 +2004,7 @@
         <v>23339</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>50</v>
       </c>
@@ -1998,7 +2036,7 @@
         <v>24069</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>100</v>
       </c>
@@ -2030,7 +2068,7 @@
         <v>26986</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>150</v>
       </c>
@@ -2062,7 +2100,7 @@
         <v>28963</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>300</v>
       </c>
@@ -2106,7 +2144,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2118,7 +2156,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agregaron archivos de ejecuciones y excel actualizados.
</commit_message>
<xml_diff>
--- a/TP2/GráficosPolinomios.xlsx
+++ b/TP2/GráficosPolinomios.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaqu\Desktop\ProgramacionAvanzada\PrograAvanzadaClaseTp\TP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laboratorios\Desktop\Ejecuciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -65,7 +65,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -78,17 +78,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -176,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -186,8 +175,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -208,7 +198,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -257,26 +247,23 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$E$3:$E$8</c:f>
+              <c:f>Hoja1!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -284,27 +271,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$3:$B$8</c:f>
+              <c:f>Hoja1!$B$3:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>20421</c:v>
+                  <c:v>3849</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25892</c:v>
+                  <c:v>3849</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51419</c:v>
+                  <c:v>4276</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>162925</c:v>
+                  <c:v>4277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>205310</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>720956</c:v>
+                  <c:v>4705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -348,26 +332,23 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$E$3:$E$8</c:f>
+              <c:f>Hoja1!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -375,27 +356,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$3:$D$8</c:f>
+              <c:f>Hoja1!$D$3:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18233</c:v>
+                  <c:v>4276</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19327</c:v>
+                  <c:v>5132</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45584</c:v>
+                  <c:v>5560</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>151339</c:v>
+                  <c:v>5559</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>167059</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>180512</c:v>
+                  <c:v>6414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -439,26 +417,23 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$E$3:$E$8</c:f>
+              <c:f>Hoja1!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -466,28 +441,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$F$3:$F$8</c:f>
+              <c:f>Hoja1!$F$3:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>16775</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24069</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>75487</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>277879</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>416455</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>777845</c:v>
-                </c:pt>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -530,26 +487,23 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$E$3:$E$8</c:f>
+              <c:f>Hoja1!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -557,28 +511,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$3:$H$8</c:f>
+              <c:f>Hoja1!$H$3:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>63293</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>68923</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66735</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>129094</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>153999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>130188</c:v>
-                </c:pt>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -621,26 +557,23 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$E$3:$E$8</c:f>
+              <c:f>Hoja1!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -648,28 +581,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$J$3:$J$8</c:f>
+              <c:f>Hoja1!$J$3:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>25527</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>23339</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>24069</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>26986</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>28963</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>29527</c:v>
-                </c:pt>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -726,6 +641,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -851,6 +767,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1521,15 +1438,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>93381</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>96369</xdr:rowOff>
+      <xdr:colOff>226731</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>58269</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>269875</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>403225</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1558,7 +1475,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1633,23 +1550,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1685,23 +1585,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1878,258 +1761,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="7" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="9"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>20421</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>18233</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>16775</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2">
-        <v>63293</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2">
-        <v>25527</v>
-      </c>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3849</v>
+      </c>
+      <c r="C3" s="9">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4276</v>
+      </c>
+      <c r="E3" s="9">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="9">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="9">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4">
-        <v>25892</v>
-      </c>
-      <c r="C4" s="10">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4">
-        <v>19327</v>
-      </c>
-      <c r="E4" s="10">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4">
-        <v>24069</v>
-      </c>
-      <c r="G4" s="10">
-        <v>10</v>
-      </c>
-      <c r="H4" s="4">
-        <v>68923</v>
-      </c>
-      <c r="I4" s="10">
-        <v>10</v>
-      </c>
-      <c r="J4" s="4">
-        <v>23339</v>
-      </c>
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3849</v>
+      </c>
+      <c r="C4" s="2">
+        <v>50</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5132</v>
+      </c>
+      <c r="E4" s="2">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2">
+        <v>50</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="2">
+        <v>50</v>
+      </c>
+      <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>50</v>
-      </c>
-      <c r="B5" s="4">
-        <v>51419</v>
-      </c>
-      <c r="C5" s="3">
-        <v>50</v>
-      </c>
-      <c r="D5" s="4">
-        <v>45584</v>
-      </c>
-      <c r="E5" s="3">
-        <v>50</v>
-      </c>
-      <c r="F5" s="4">
-        <v>75487</v>
-      </c>
-      <c r="G5" s="3">
-        <v>50</v>
-      </c>
-      <c r="H5" s="4">
-        <v>66735</v>
-      </c>
-      <c r="I5" s="3">
-        <v>50</v>
-      </c>
-      <c r="J5" s="4">
-        <v>24069</v>
-      </c>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4276</v>
+      </c>
+      <c r="C5" s="2">
+        <v>100</v>
+      </c>
+      <c r="D5" s="10">
+        <v>5560</v>
+      </c>
+      <c r="E5" s="2">
+        <v>100</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="2">
+        <v>100</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="2">
+        <v>100</v>
+      </c>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>100</v>
-      </c>
-      <c r="B6" s="4">
-        <v>162925</v>
-      </c>
-      <c r="C6" s="3">
-        <v>100</v>
-      </c>
-      <c r="D6" s="4">
-        <v>151339</v>
-      </c>
-      <c r="E6" s="3">
-        <v>100</v>
-      </c>
-      <c r="F6" s="4">
-        <v>277879</v>
-      </c>
-      <c r="G6" s="3">
-        <v>100</v>
-      </c>
-      <c r="H6" s="4">
-        <v>129094</v>
-      </c>
-      <c r="I6" s="3">
-        <v>100</v>
-      </c>
-      <c r="J6" s="4">
-        <v>26986</v>
-      </c>
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4277</v>
+      </c>
+      <c r="C6" s="2">
+        <v>150</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5559</v>
+      </c>
+      <c r="E6" s="2">
+        <v>150</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="2">
+        <v>150</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="2">
+        <v>150</v>
+      </c>
+      <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>150</v>
-      </c>
-      <c r="B7" s="4">
-        <v>205310</v>
-      </c>
-      <c r="C7" s="3">
-        <v>150</v>
-      </c>
-      <c r="D7" s="4">
-        <v>167059</v>
-      </c>
-      <c r="E7" s="3">
-        <v>150</v>
-      </c>
-      <c r="F7" s="4">
-        <v>416455</v>
-      </c>
-      <c r="G7" s="3">
-        <v>150</v>
-      </c>
-      <c r="H7" s="4">
-        <v>153999</v>
-      </c>
-      <c r="I7" s="3">
-        <v>150</v>
-      </c>
-      <c r="J7" s="4">
-        <v>28963</v>
-      </c>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4705</v>
+      </c>
+      <c r="C7" s="4">
+        <v>300</v>
+      </c>
+      <c r="D7" s="5">
+        <v>6414</v>
+      </c>
+      <c r="E7" s="4">
+        <v>300</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="4">
+        <v>300</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="4">
+        <v>300</v>
+      </c>
+      <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>300</v>
-      </c>
-      <c r="B8" s="6">
-        <v>720956</v>
-      </c>
-      <c r="C8" s="5">
-        <v>300</v>
-      </c>
-      <c r="D8" s="6">
-        <v>180512</v>
-      </c>
-      <c r="E8" s="5">
-        <v>300</v>
-      </c>
-      <c r="F8" s="6">
-        <v>777845</v>
-      </c>
-      <c r="G8" s="5">
-        <v>300</v>
-      </c>
-      <c r="H8" s="6">
-        <v>130188</v>
-      </c>
-      <c r="I8" s="5">
-        <v>300</v>
-      </c>
-      <c r="J8" s="6">
-        <v>29527</v>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11">
+        <v>4704</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>5987</v>
+      </c>
+      <c r="C9" s="9">
+        <v>9</v>
+      </c>
+      <c r="E9" s="9">
+        <v>9</v>
+      </c>
+      <c r="G9" s="9">
+        <v>9</v>
+      </c>
+      <c r="I9" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>6415</v>
+      </c>
+      <c r="C10" s="10">
+        <v>10</v>
+      </c>
+      <c r="E10" s="10">
+        <v>10</v>
+      </c>
+      <c r="G10" s="10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>14112</v>
+      </c>
+      <c r="C11" s="10">
+        <v>20</v>
+      </c>
+      <c r="E11" s="10">
+        <v>20</v>
+      </c>
+      <c r="G11" s="10">
+        <v>20</v>
+      </c>
+      <c r="I11" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>29081</v>
+      </c>
+      <c r="C12" s="10">
+        <v>30</v>
+      </c>
+      <c r="E12" s="10">
+        <v>30</v>
+      </c>
+      <c r="G12" s="10">
+        <v>30</v>
+      </c>
+      <c r="I12" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>56878</v>
+      </c>
+      <c r="C13" s="10">
+        <v>40</v>
+      </c>
+      <c r="E13" s="10">
+        <v>40</v>
+      </c>
+      <c r="G13" s="10">
+        <v>40</v>
+      </c>
+      <c r="I13" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>128724</v>
+      </c>
+      <c r="C14" s="10">
+        <v>50</v>
+      </c>
+      <c r="E14" s="10">
+        <v>50</v>
+      </c>
+      <c r="G14" s="10">
+        <v>50</v>
+      </c>
+      <c r="I14" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>94512</v>
+      </c>
+      <c r="C15" s="10">
+        <v>60</v>
+      </c>
+      <c r="E15" s="10">
+        <v>60</v>
+      </c>
+      <c r="G15" s="10">
+        <v>60</v>
+      </c>
+      <c r="I15" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>70</v>
+      </c>
+      <c r="B16">
+        <v>132145</v>
+      </c>
+      <c r="C16" s="10">
+        <v>70</v>
+      </c>
+      <c r="E16" s="10">
+        <v>70</v>
+      </c>
+      <c r="G16" s="10">
+        <v>70</v>
+      </c>
+      <c r="I16" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>159088</v>
+      </c>
+      <c r="C17" s="10">
+        <v>80</v>
+      </c>
+      <c r="E17" s="10">
+        <v>80</v>
+      </c>
+      <c r="G17" s="10">
+        <v>80</v>
+      </c>
+      <c r="I17" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>90</v>
+      </c>
+      <c r="B18">
+        <v>211262</v>
+      </c>
+      <c r="C18" s="10">
+        <v>90</v>
+      </c>
+      <c r="E18" s="10">
+        <v>90</v>
+      </c>
+      <c r="G18" s="10">
+        <v>90</v>
+      </c>
+      <c r="I18" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>200</v>
+      </c>
+      <c r="B19">
+        <v>977192</v>
+      </c>
+      <c r="C19" s="10">
+        <v>200</v>
+      </c>
+      <c r="E19" s="10">
+        <v>200</v>
+      </c>
+      <c r="G19" s="10">
+        <v>200</v>
+      </c>
+      <c r="I19" s="10">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2144,7 +2205,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2156,7 +2217,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>